<commit_message>
submit 9 script by zoe
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/Keywordscripts/600.40.10.20_UserAndGroupAUserWithoutForwardTrapConfigure.xlsx
+++ b/NformTester/NformTester/Keywordscripts/600.40.10.20_UserAndGroupAUserWithoutForwardTrapConfigure.xlsx
@@ -4706,8 +4706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I51" sqref="I51"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>